<commit_message>
Fixed a bug due to not cleaning the program parameters.
</commit_message>
<xml_diff>
--- a/tests/data/tables/real.RMS1-G02.xlsx
+++ b/tests/data/tables/real.RMS1-G02.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="trajectory" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">Trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seqId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position</t>
+  </si>
   <si>
     <t xml:space="preserve">RMS1-G02</t>
   </si>
@@ -77,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -342,7 +352,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -351,9 +361,15 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="3" t="n">
         <v>0</v>
       </c>
@@ -393,10 +409,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>45353</v>
@@ -440,10 +456,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8" t="n">
         <v>64422</v>
@@ -487,10 +503,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>517531</v>
@@ -534,10 +550,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>555199</v>
@@ -581,10 +597,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>813080</v>
@@ -628,10 +644,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>56843</v>
@@ -675,10 +691,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>311513</v>
@@ -722,10 +738,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>196851</v>
@@ -769,10 +785,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>303485</v>
@@ -816,10 +832,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>716752</v>
@@ -863,10 +879,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8" t="n">
         <v>799769</v>
@@ -910,10 +926,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" s="8" t="n">
         <v>1469971</v>
@@ -957,10 +973,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14" s="8" t="n">
         <v>132435</v>
@@ -1004,10 +1020,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" s="8" t="n">
         <v>611943</v>
@@ -1051,10 +1067,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8" t="n">
         <v>713295</v>
@@ -1098,10 +1114,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C17" s="8" t="n">
         <v>902982</v>
@@ -1145,10 +1161,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" s="8" t="n">
         <v>1038759</v>
@@ -1192,10 +1208,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>275590</v>
@@ -1239,10 +1255,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="8" t="n">
         <v>353766</v>
@@ -1286,10 +1302,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="8" t="n">
         <v>416864</v>
@@ -1333,10 +1349,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C22" s="8" t="n">
         <v>463844</v>
@@ -1380,10 +1396,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C23" s="8" t="n">
         <v>136049</v>
@@ -1427,10 +1443,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8" t="n">
         <v>152173</v>
@@ -1474,10 +1490,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C25" s="8" t="n">
         <v>526317</v>
@@ -1521,10 +1537,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C26" s="8" t="n">
         <v>950119</v>
@@ -1568,10 +1584,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C27" s="8" t="n">
         <v>952467</v>
@@ -1615,10 +1631,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>410284</v>
@@ -1662,10 +1678,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C29" s="8" t="n">
         <v>514803</v>
@@ -1709,10 +1725,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C30" s="8" t="n">
         <v>894013</v>
@@ -1756,10 +1772,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C31" s="8" t="n">
         <v>302526</v>
@@ -1803,10 +1819,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C32" s="8" t="n">
         <v>574533</v>
@@ -1850,10 +1866,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C33" s="8" t="n">
         <v>302177</v>
@@ -1897,10 +1913,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C34" s="8" t="n">
         <v>390550</v>
@@ -1944,10 +1960,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C35" s="11" t="n">
         <v>663757</v>

</xml_diff>